<commit_message>
v 1.0.0 packagedown built
</commit_message>
<xml_diff>
--- a/vignettes/outtable.xlsx
+++ b/vignettes/outtable.xlsx
@@ -48,10 +48,10 @@
     <t xml:space="preserve">Example Table</t>
   </si>
   <si>
-    <t xml:space="preserve">Generated By: \\pfs1w\C:\Users\kheal579\Documents\01_integral-private\integral-private\vignettes\C:\Users\kheal579\AppData\Local\Temp\RtmpWuRGVr\callr-scr-740416df42b</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Created By: Eben Pendleton on 2022-08-15</t>
+    <t xml:space="preserve">Generated By: \\pfs1w\C:\Users\kheal579\Documents\01_integral-private\integral-private\vignettes\C:\Users\kheal579\AppData\Local\Temp\Rtmp2nWN2H\callr-scr-99a4716e1e26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Created By: Eben Pendleton on 2022-08-24</t>
   </si>
 </sst>
 </file>

</xml_diff>